<commit_message>
Update doc. Last version of mgr doc.
</commit_message>
<xml_diff>
--- a/docs/results/mgrNumbers.xlsx
+++ b/docs/results/mgrNumbers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloud\Dropbox\Public\MolecularDynamics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\MolecularDynamics\docs\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1815" windowWidth="23445" windowHeight="9795" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="2265" windowWidth="23445" windowHeight="9795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LJ" sheetId="1" r:id="rId1"/>
@@ -452,11 +452,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1438645200"/>
-        <c:axId val="1438657712"/>
+        <c:axId val="420889184"/>
+        <c:axId val="420878304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1438645200"/>
+        <c:axId val="420889184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -488,7 +488,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1438657712"/>
+        <c:crossAx val="420878304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -496,7 +496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438657712"/>
+        <c:axId val="420878304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="10"/>
@@ -527,7 +527,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1438645200"/>
+        <c:crossAx val="420889184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -822,11 +822,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1440952752"/>
-        <c:axId val="1440962544"/>
+        <c:axId val="552826128"/>
+        <c:axId val="553814624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1440952752"/>
+        <c:axId val="552826128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -906,7 +906,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440962544"/>
+        <c:crossAx val="553814624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -914,7 +914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440962544"/>
+        <c:axId val="553814624"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1014,7 +1014,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440952752"/>
+        <c:crossAx val="552826128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1169,7 +1169,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Przyspieszenie</a:t>
+              <a:t>Wzrost efektywności</a:t>
             </a:r>
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
@@ -1195,7 +1195,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Przyspieszenie</c:v>
+            <c:v>Efektywność</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1340,11 +1340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1440961456"/>
-        <c:axId val="1440948944"/>
+        <c:axId val="553816256"/>
+        <c:axId val="553826048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1440961456"/>
+        <c:axId val="553816256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,7 +1424,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440948944"/>
+        <c:crossAx val="553826048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1432,7 +1432,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440948944"/>
+        <c:axId val="553826048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1520,7 +1520,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440961456"/>
+        <c:crossAx val="553816256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1863,11 +1863,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1440955472"/>
-        <c:axId val="1440956560"/>
+        <c:axId val="553812448"/>
+        <c:axId val="553815168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1440955472"/>
+        <c:axId val="553812448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1947,7 +1947,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440956560"/>
+        <c:crossAx val="553815168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1955,7 +1955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440956560"/>
+        <c:axId val="553815168"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -2044,7 +2044,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440955472"/>
+        <c:crossAx val="553812448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2389,11 +2389,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1441225712"/>
-        <c:axId val="1441227344"/>
+        <c:axId val="553827136"/>
+        <c:axId val="553825504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1441225712"/>
+        <c:axId val="553827136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2477,7 +2477,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1441227344"/>
+        <c:crossAx val="553825504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2485,7 +2485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1441227344"/>
+        <c:axId val="553825504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,7 +2573,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1441225712"/>
+        <c:crossAx val="553827136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2856,11 +2856,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1256808720"/>
-        <c:axId val="1256816880"/>
+        <c:axId val="553824960"/>
+        <c:axId val="553819520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1256808720"/>
+        <c:axId val="553824960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2964,7 +2964,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1256816880"/>
+        <c:crossAx val="553819520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2972,7 +2972,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1256816880"/>
+        <c:axId val="553819520"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3081,7 +3081,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1256808720"/>
+        <c:crossAx val="553824960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3336,11 +3336,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1443591600"/>
-        <c:axId val="1443597040"/>
+        <c:axId val="553826592"/>
+        <c:axId val="553816800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1443591600"/>
+        <c:axId val="553826592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3440,7 +3440,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1443597040"/>
+        <c:crossAx val="553816800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3448,7 +3448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1443597040"/>
+        <c:axId val="553816800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -3561,7 +3561,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1443591600"/>
+        <c:crossAx val="553826592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3757,11 +3757,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1483865776"/>
-        <c:axId val="1483872848"/>
+        <c:axId val="553818432"/>
+        <c:axId val="553818976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1483865776"/>
+        <c:axId val="553818432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3861,7 +3861,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1483872848"/>
+        <c:crossAx val="553818976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3869,7 +3869,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1483872848"/>
+        <c:axId val="553818976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2"/>
@@ -3979,7 +3979,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1483865776"/>
+        <c:crossAx val="553818432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4350,11 +4350,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1438656624"/>
-        <c:axId val="1438647376"/>
+        <c:axId val="420892992"/>
+        <c:axId val="420883200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1438656624"/>
+        <c:axId val="420892992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4433,7 +4433,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438647376"/>
+        <c:crossAx val="420883200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4441,7 +4441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438647376"/>
+        <c:axId val="420883200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4532,7 +4532,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438656624"/>
+        <c:crossAx val="420892992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4906,11 +4906,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1438653360"/>
-        <c:axId val="1438654992"/>
+        <c:axId val="420882112"/>
+        <c:axId val="420886464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1438653360"/>
+        <c:axId val="420882112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4989,7 +4989,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438654992"/>
+        <c:crossAx val="420886464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4997,7 +4997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438654992"/>
+        <c:axId val="420886464"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -5087,7 +5087,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438653360"/>
+        <c:crossAx val="420882112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5430,11 +5430,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1438646832"/>
-        <c:axId val="1438647920"/>
+        <c:axId val="419191776"/>
+        <c:axId val="552829936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1438646832"/>
+        <c:axId val="419191776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5513,7 +5513,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438647920"/>
+        <c:crossAx val="552829936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5521,7 +5521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438647920"/>
+        <c:axId val="552829936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5620,7 +5620,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438646832"/>
+        <c:crossAx val="419191776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6017,11 +6017,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1438644112"/>
-        <c:axId val="1438649552"/>
+        <c:axId val="552828848"/>
+        <c:axId val="552820688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1438644112"/>
+        <c:axId val="552828848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6064,7 +6064,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438649552"/>
+        <c:crossAx val="552820688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6072,7 +6072,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1438649552"/>
+        <c:axId val="552820688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="10"/>
@@ -6124,7 +6124,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1438644112"/>
+        <c:crossAx val="552828848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6459,11 +6459,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1277659616"/>
-        <c:axId val="1277650368"/>
+        <c:axId val="552831024"/>
+        <c:axId val="552831568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1277659616"/>
+        <c:axId val="552831024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6542,7 +6542,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277650368"/>
+        <c:crossAx val="552831568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6550,7 +6550,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1277650368"/>
+        <c:axId val="552831568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6649,7 +6649,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1277659616"/>
+        <c:crossAx val="552831024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7031,11 +7031,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1440958192"/>
-        <c:axId val="1440952208"/>
+        <c:axId val="552829392"/>
+        <c:axId val="552827760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1440958192"/>
+        <c:axId val="552829392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7114,7 +7114,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440952208"/>
+        <c:crossAx val="552827760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7122,7 +7122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440952208"/>
+        <c:axId val="552827760"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7218,7 +7218,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440958192"/>
+        <c:crossAx val="552829392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7600,11 +7600,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1440959824"/>
-        <c:axId val="1440951664"/>
+        <c:axId val="552826672"/>
+        <c:axId val="552819056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1440959824"/>
+        <c:axId val="552826672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7683,7 +7683,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440951664"/>
+        <c:crossAx val="552819056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7691,7 +7691,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440951664"/>
+        <c:axId val="552819056"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -7791,7 +7791,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440959824"/>
+        <c:crossAx val="552826672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8166,11 +8166,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1440963088"/>
-        <c:axId val="1440960368"/>
+        <c:axId val="552830480"/>
+        <c:axId val="552820144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1440963088"/>
+        <c:axId val="552830480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8250,7 +8250,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440960368"/>
+        <c:crossAx val="552820144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8258,7 +8258,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1440960368"/>
+        <c:axId val="552820144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8357,7 +8357,7 @@
             <a:endParaRPr lang="pl-PL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1440963088"/>
+        <c:crossAx val="552830480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11160,7 +11160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J108"/>
   <sheetViews>
-    <sheetView topLeftCell="B94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B94" workbookViewId="0">
       <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
@@ -11957,7 +11957,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>

</xml_diff>